<commit_message>
updating code to analyze Shuffled Image data
successfully updated errorTrialsPerTeaskfile, preprocessinf_steps; started updating grasp_decoding, tuning_analysis, plot_firing_rates; focusing on tuning_analysis
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_4S_Action.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_4S_Action.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09B7688-A140-4813-A3A8-F1F011015FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684A3DE-7999-41A2-83E3-AA7EA54088F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4470" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2310" yWindow="0" windowWidth="12150" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -35,6 +35,75 @@
   </si>
   <si>
     <t>Grasps_Object'</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>10,13,14</t>
+  </si>
+  <si>
+    <t>14,18</t>
+  </si>
+  <si>
+    <t>9,20</t>
+  </si>
+  <si>
+    <t>14,18,19,20</t>
+  </si>
+  <si>
+    <t>17,18,19,20</t>
+  </si>
+  <si>
+    <t>1,3,1,2,3,2</t>
+  </si>
+  <si>
+    <t>13,16,17,18,19</t>
+  </si>
+  <si>
+    <t>8,9,18</t>
+  </si>
+  <si>
+    <t>19,20</t>
+  </si>
+  <si>
+    <t>9,18,20</t>
+  </si>
+  <si>
+    <t>18,19</t>
+  </si>
+  <si>
+    <t>5,16,17</t>
+  </si>
+  <si>
+    <t>2,1,3,2,1,3</t>
+  </si>
+  <si>
+    <t>3,18</t>
+  </si>
+  <si>
+    <t>12,13,14</t>
+  </si>
+  <si>
+    <t>7,18</t>
+  </si>
+  <si>
+    <t>2,3,1,2,3,1</t>
+  </si>
+  <si>
+    <t>3,7,12,13,17,18,19</t>
+  </si>
+  <si>
+    <t>2,4,5,8,9,10,15,16</t>
+  </si>
+  <si>
+    <t>13,19,20</t>
+  </si>
+  <si>
+    <t>6,13,14,19</t>
+  </si>
+  <si>
+    <t>7,13</t>
   </si>
 </sst>
 </file>
@@ -353,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +513,229 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20230921</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20230922</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20231016</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20231101</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20231103</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20231201</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated tuning analyses across participants, worked on tuning code (commenting and determining effect sizes)
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_4S_Action.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_4S_Action.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684A3DE-7999-41A2-83E3-AA7EA54088F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7EC114-C78C-4077-84B0-FF8D19A527F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="0" windowWidth="12150" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15240" yWindow="3000" windowWidth="15420" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>7,13</t>
+  </si>
+  <si>
+    <t>excluded</t>
   </si>
 </sst>
 </file>
@@ -424,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +604,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20231101</v>

</xml_diff>